<commit_message>
Add source emebed, remove duplicated code, try .mobile for graph1
</commit_message>
<xml_diff>
--- a/data/COVID-19CumulativeTestTotalsbyCounty.xlsx
+++ b/data/COVID-19CumulativeTestTotalsbyCounty.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BEF50DA8-CE60-40D6-ACDF-D28E0FA0B6DE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A07F3D26-A78C-4F2A-A140-8401D1A89E77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="345">
   <si>
     <t>County</t>
   </si>
@@ -1061,7 +1061,10 @@
     <t>Tests Through July 5</t>
   </si>
   <si>
-    <t>5. This file will be updated daily; the next cumulative update will be 7/7/2020.</t>
+    <t>Tests Through July 6</t>
+  </si>
+  <si>
+    <t>5. This file will be updated daily; the next cumulative update will be 7/8/2020.</t>
   </si>
 </sst>
 </file>
@@ -1510,13 +1513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BY267"/>
+  <dimension ref="A1:BZ267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A267" sqref="A267:I267"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1528,15 +1531,15 @@
     <col min="46" max="46" width="11.453125" style="2" customWidth="1"/>
     <col min="47" max="49" width="11.1796875" style="2" customWidth="1"/>
     <col min="50" max="71" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="72" max="77" width="11.08984375" customWidth="1"/>
+    <col min="72" max="78" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:77" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:78" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1768,8 +1771,11 @@
       <c r="BY2" s="7" t="s">
         <v>342</v>
       </c>
+      <c r="BZ2" s="7" t="s">
+        <v>343</v>
+      </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -2001,8 +2007,11 @@
       <c r="BY3" s="2">
         <v>11037</v>
       </c>
+      <c r="BZ3" s="2">
+        <v>11081</v>
+      </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2234,8 +2243,11 @@
       <c r="BY4">
         <v>169</v>
       </c>
+      <c r="BZ4">
+        <v>184</v>
+      </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -2467,8 +2479,11 @@
       <c r="BY5" s="2">
         <v>4821</v>
       </c>
+      <c r="BZ5" s="2">
+        <v>4962</v>
+      </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2700,8 +2715,11 @@
       <c r="BY6">
         <v>433</v>
       </c>
+      <c r="BZ6">
+        <v>450</v>
+      </c>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2933,8 +2951,11 @@
       <c r="BY7">
         <v>107</v>
       </c>
+      <c r="BZ7">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -3166,8 +3187,11 @@
       <c r="BY8">
         <v>188</v>
       </c>
+      <c r="BZ8">
+        <v>189</v>
+      </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -3399,8 +3423,11 @@
       <c r="BY9" s="2">
         <v>2050</v>
       </c>
+      <c r="BZ9" s="2">
+        <v>2107</v>
+      </c>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -3632,8 +3659,11 @@
       <c r="BY10" s="2">
         <v>1852</v>
       </c>
+      <c r="BZ10" s="2">
+        <v>1882</v>
+      </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -3865,8 +3895,11 @@
       <c r="BY11">
         <v>134</v>
       </c>
+      <c r="BZ11">
+        <v>134</v>
+      </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -4098,8 +4131,11 @@
       <c r="BY12">
         <v>535</v>
       </c>
+      <c r="BZ12">
+        <v>551</v>
+      </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -4331,8 +4367,11 @@
       <c r="BY13" s="2">
         <v>2976</v>
       </c>
+      <c r="BZ13" s="2">
+        <v>3073</v>
+      </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -4564,8 +4603,11 @@
       <c r="BY14">
         <v>76</v>
       </c>
+      <c r="BZ14">
+        <v>80</v>
+      </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -4797,8 +4839,11 @@
       <c r="BY15" s="2">
         <v>4642</v>
       </c>
+      <c r="BZ15" s="2">
+        <v>4676</v>
+      </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -5030,8 +5075,11 @@
       <c r="BY16" s="2">
         <v>24738</v>
       </c>
+      <c r="BZ16" s="2">
+        <v>24958</v>
+      </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -5263,8 +5311,11 @@
       <c r="BY17" s="2">
         <v>91707</v>
       </c>
+      <c r="BZ17" s="2">
+        <v>94612</v>
+      </c>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -5496,8 +5547,11 @@
       <c r="BY18" s="2">
         <v>2889</v>
       </c>
+      <c r="BZ18" s="2">
+        <v>2954</v>
+      </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -5729,8 +5783,11 @@
       <c r="BY19">
         <v>2</v>
       </c>
+      <c r="BZ19">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
@@ -5962,8 +6019,11 @@
       <c r="BY20" s="2">
         <v>1074</v>
       </c>
+      <c r="BZ20" s="2">
+        <v>1081</v>
+      </c>
     </row>
-    <row r="21" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -6195,8 +6255,11 @@
       <c r="BY21" s="2">
         <v>8142</v>
       </c>
+      <c r="BZ21" s="2">
+        <v>8222</v>
+      </c>
     </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -6428,8 +6491,11 @@
       <c r="BY22" s="2">
         <v>21333</v>
       </c>
+      <c r="BZ22" s="2">
+        <v>21931</v>
+      </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
@@ -6661,8 +6727,11 @@
       <c r="BY23" s="2">
         <v>15564</v>
       </c>
+      <c r="BZ23" s="2">
+        <v>15739</v>
+      </c>
     </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
@@ -6894,8 +6963,11 @@
       <c r="BY24">
         <v>1033</v>
       </c>
+      <c r="BZ24">
+        <v>1050</v>
+      </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
@@ -7127,8 +7199,11 @@
       <c r="BY25">
         <v>75</v>
       </c>
+      <c r="BZ25">
+        <v>90</v>
+      </c>
     </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -7360,8 +7435,11 @@
       <c r="BY26">
         <v>176</v>
       </c>
+      <c r="BZ26">
+        <v>179</v>
+      </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
@@ -7593,8 +7671,11 @@
       <c r="BY27" s="2">
         <v>1253</v>
       </c>
+      <c r="BZ27" s="2">
+        <v>1297</v>
+      </c>
     </row>
-    <row r="28" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -7826,8 +7907,11 @@
       <c r="BY28">
         <v>888</v>
       </c>
+      <c r="BZ28">
+        <v>921</v>
+      </c>
     </row>
-    <row r="29" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
@@ -8059,8 +8143,11 @@
       <c r="BY29" s="2">
         <v>2068</v>
       </c>
+      <c r="BZ29" s="2">
+        <v>2177</v>
+      </c>
     </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
@@ -8292,8 +8379,11 @@
       <c r="BY30" s="2">
         <v>1858</v>
       </c>
+      <c r="BZ30" s="2">
+        <v>1998</v>
+      </c>
     </row>
-    <row r="31" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
@@ -8525,8 +8615,11 @@
       <c r="BY31" s="2">
         <v>1237</v>
       </c>
+      <c r="BZ31" s="2">
+        <v>1247</v>
+      </c>
     </row>
-    <row r="32" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>30</v>
       </c>
@@ -8758,8 +8851,11 @@
       <c r="BY32">
         <v>380</v>
       </c>
+      <c r="BZ32">
+        <v>392</v>
+      </c>
     </row>
-    <row r="33" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>31</v>
       </c>
@@ -8991,8 +9087,11 @@
       <c r="BY33" s="2">
         <v>23576</v>
       </c>
+      <c r="BZ33" s="2">
+        <v>24273</v>
+      </c>
     </row>
-    <row r="34" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>32</v>
       </c>
@@ -9224,8 +9323,11 @@
       <c r="BY34">
         <v>408</v>
       </c>
+      <c r="BZ34">
+        <v>422</v>
+      </c>
     </row>
-    <row r="35" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>33</v>
       </c>
@@ -9457,8 +9559,11 @@
       <c r="BY35">
         <v>199</v>
       </c>
+      <c r="BZ35">
+        <v>204</v>
+      </c>
     </row>
-    <row r="36" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
@@ -9690,8 +9795,11 @@
       <c r="BY36">
         <v>948</v>
       </c>
+      <c r="BZ36">
+        <v>958</v>
+      </c>
     </row>
-    <row r="37" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
@@ -9923,8 +10031,11 @@
       <c r="BY37">
         <v>340</v>
       </c>
+      <c r="BZ37">
+        <v>340</v>
+      </c>
     </row>
-    <row r="38" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>36</v>
       </c>
@@ -10156,8 +10267,11 @@
       <c r="BY38" s="2">
         <v>2685</v>
       </c>
+      <c r="BZ38" s="2">
+        <v>2810</v>
+      </c>
     </row>
-    <row r="39" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>37</v>
       </c>
@@ -10389,8 +10503,11 @@
       <c r="BY39" s="2">
         <v>2959</v>
       </c>
+      <c r="BZ39" s="2">
+        <v>2997</v>
+      </c>
     </row>
-    <row r="40" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>38</v>
       </c>
@@ -10622,8 +10739,11 @@
       <c r="BY40">
         <v>319</v>
       </c>
+      <c r="BZ40">
+        <v>322</v>
+      </c>
     </row>
-    <row r="41" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
@@ -10855,8 +10975,11 @@
       <c r="BY41">
         <v>356</v>
       </c>
+      <c r="BZ41">
+        <v>366</v>
+      </c>
     </row>
-    <row r="42" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
@@ -11088,8 +11211,11 @@
       <c r="BY42">
         <v>27</v>
       </c>
+      <c r="BZ42">
+        <v>29</v>
+      </c>
     </row>
-    <row r="43" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>41</v>
       </c>
@@ -11321,8 +11447,11 @@
       <c r="BY43">
         <v>41</v>
       </c>
+      <c r="BZ43">
+        <v>43</v>
+      </c>
     </row>
-    <row r="44" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>42</v>
       </c>
@@ -11554,8 +11683,11 @@
       <c r="BY44">
         <v>223</v>
       </c>
+      <c r="BZ44">
+        <v>236</v>
+      </c>
     </row>
-    <row r="45" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -11787,8 +11919,11 @@
       <c r="BY45" s="2">
         <v>52116</v>
       </c>
+      <c r="BZ45" s="2">
+        <v>52850</v>
+      </c>
     </row>
-    <row r="46" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>44</v>
       </c>
@@ -12020,8 +12155,11 @@
       <c r="BY46">
         <v>169</v>
       </c>
+      <c r="BZ46">
+        <v>169</v>
+      </c>
     </row>
-    <row r="47" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>45</v>
       </c>
@@ -12253,8 +12391,11 @@
       <c r="BY47" s="2">
         <v>1357</v>
       </c>
+      <c r="BZ47" s="2">
+        <v>1372</v>
+      </c>
     </row>
-    <row r="48" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>46</v>
       </c>
@@ -12486,8 +12627,11 @@
       <c r="BY48" s="2">
         <v>7200</v>
       </c>
+      <c r="BZ48" s="2">
+        <v>7369</v>
+      </c>
     </row>
-    <row r="49" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
@@ -12719,8 +12863,11 @@
       <c r="BY49">
         <v>812</v>
       </c>
+      <c r="BZ49">
+        <v>819</v>
+      </c>
     </row>
-    <row r="50" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
@@ -12952,8 +13099,11 @@
       <c r="BY50">
         <v>110</v>
       </c>
+      <c r="BZ50">
+        <v>111</v>
+      </c>
     </row>
-    <row r="51" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>49</v>
       </c>
@@ -13185,8 +13335,11 @@
       <c r="BY51" s="2">
         <v>1995</v>
       </c>
+      <c r="BZ51" s="2">
+        <v>2040</v>
+      </c>
     </row>
-    <row r="52" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>50</v>
       </c>
@@ -13418,8 +13571,11 @@
       <c r="BY52" s="2">
         <v>11061</v>
       </c>
+      <c r="BZ52" s="2">
+        <v>11080</v>
+      </c>
     </row>
-    <row r="53" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
@@ -13651,8 +13807,11 @@
       <c r="BY53">
         <v>41</v>
       </c>
+      <c r="BZ53">
+        <v>42</v>
+      </c>
     </row>
-    <row r="54" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>52</v>
       </c>
@@ -13884,8 +14043,11 @@
       <c r="BY54">
         <v>213</v>
       </c>
+      <c r="BZ54">
+        <v>216</v>
+      </c>
     </row>
-    <row r="55" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>53</v>
       </c>
@@ -14117,8 +14279,11 @@
       <c r="BY55">
         <v>124</v>
       </c>
+      <c r="BZ55">
+        <v>124</v>
+      </c>
     </row>
-    <row r="56" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>54</v>
       </c>
@@ -14350,8 +14515,11 @@
       <c r="BY56">
         <v>174</v>
       </c>
+      <c r="BZ56">
+        <v>176</v>
+      </c>
     </row>
-    <row r="57" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>55</v>
       </c>
@@ -14583,8 +14751,11 @@
       <c r="BY57">
         <v>63</v>
       </c>
+      <c r="BZ57">
+        <v>65</v>
+      </c>
     </row>
-    <row r="58" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>56</v>
       </c>
@@ -14816,8 +14987,11 @@
       <c r="BY58">
         <v>10</v>
       </c>
+      <c r="BZ58">
+        <v>10</v>
+      </c>
     </row>
-    <row r="59" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
@@ -15049,8 +15223,11 @@
       <c r="BY59" s="2">
         <v>204605</v>
       </c>
+      <c r="BZ59" s="2">
+        <v>208058</v>
+      </c>
     </row>
-    <row r="60" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
@@ -15282,8 +15459,11 @@
       <c r="BY60">
         <v>1910</v>
       </c>
+      <c r="BZ60">
+        <v>1910</v>
+      </c>
     </row>
-    <row r="61" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>59</v>
       </c>
@@ -15515,8 +15695,11 @@
       <c r="BY61">
         <v>506</v>
       </c>
+      <c r="BZ61">
+        <v>510</v>
+      </c>
     </row>
-    <row r="62" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>60</v>
       </c>
@@ -15748,8 +15931,11 @@
       <c r="BY62">
         <v>115</v>
       </c>
+      <c r="BZ62">
+        <v>116</v>
+      </c>
     </row>
-    <row r="63" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>61</v>
       </c>
@@ -15981,8 +16167,11 @@
       <c r="BY63" s="2">
         <v>46253</v>
       </c>
+      <c r="BZ63" s="2">
+        <v>47153</v>
+      </c>
     </row>
-    <row r="64" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>62</v>
       </c>
@@ -16214,8 +16403,11 @@
       <c r="BY64">
         <v>653</v>
       </c>
+      <c r="BZ64">
+        <v>719</v>
+      </c>
     </row>
-    <row r="65" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>63</v>
       </c>
@@ -16447,8 +16639,11 @@
       <c r="BY65">
         <v>32</v>
       </c>
+      <c r="BZ65">
+        <v>32</v>
+      </c>
     </row>
-    <row r="66" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>64</v>
       </c>
@@ -16680,8 +16875,11 @@
       <c r="BY66">
         <v>513</v>
       </c>
+      <c r="BZ66">
+        <v>743</v>
+      </c>
     </row>
-    <row r="67" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>65</v>
       </c>
@@ -16913,8 +17111,11 @@
       <c r="BY67">
         <v>201</v>
       </c>
+      <c r="BZ67">
+        <v>205</v>
+      </c>
     </row>
-    <row r="68" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>66</v>
       </c>
@@ -17146,8 +17347,11 @@
       <c r="BY68">
         <v>497</v>
       </c>
+      <c r="BZ68">
+        <v>532</v>
+      </c>
     </row>
-    <row r="69" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>67</v>
       </c>
@@ -17379,8 +17583,11 @@
       <c r="BY69">
         <v>515</v>
       </c>
+      <c r="BZ69">
+        <v>527</v>
+      </c>
     </row>
-    <row r="70" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>68</v>
       </c>
@@ -17612,8 +17819,11 @@
       <c r="BY70" s="2">
         <v>6138</v>
       </c>
+      <c r="BZ70" s="2">
+        <v>6421</v>
+      </c>
     </row>
-    <row r="71" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>69</v>
       </c>
@@ -17845,8 +18055,11 @@
       <c r="BY71">
         <v>40</v>
       </c>
+      <c r="BZ71">
+        <v>40</v>
+      </c>
     </row>
-    <row r="72" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>70</v>
       </c>
@@ -18078,8 +18291,11 @@
       <c r="BY72" s="2">
         <v>12117</v>
       </c>
+      <c r="BZ72" s="2">
+        <v>12477</v>
+      </c>
     </row>
-    <row r="73" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>71</v>
       </c>
@@ -18311,8 +18527,11 @@
       <c r="BY73" s="2">
         <v>48877</v>
       </c>
+      <c r="BZ73" s="2">
+        <v>50759</v>
+      </c>
     </row>
-    <row r="74" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>72</v>
       </c>
@@ -18544,8 +18763,11 @@
       <c r="BY74" s="2">
         <v>1673</v>
       </c>
+      <c r="BZ74" s="2">
+        <v>1691</v>
+      </c>
     </row>
-    <row r="75" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>73</v>
       </c>
@@ -18777,8 +18999,11 @@
       <c r="BY75">
         <v>2167</v>
       </c>
+      <c r="BZ75">
+        <v>2178</v>
+      </c>
     </row>
-    <row r="76" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>74</v>
       </c>
@@ -19010,8 +19235,11 @@
       <c r="BY76" s="2">
         <v>1739</v>
       </c>
+      <c r="BZ76" s="2">
+        <v>1756</v>
+      </c>
     </row>
-    <row r="77" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>75</v>
       </c>
@@ -19243,8 +19471,11 @@
       <c r="BY77" s="2">
         <v>1763</v>
       </c>
+      <c r="BZ77" s="2">
+        <v>1791</v>
+      </c>
     </row>
-    <row r="78" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>76</v>
       </c>
@@ -19476,8 +19707,11 @@
       <c r="BY78">
         <v>41</v>
       </c>
+      <c r="BZ78">
+        <v>41</v>
+      </c>
     </row>
-    <row r="79" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>77</v>
       </c>
@@ -19709,8 +19943,11 @@
       <c r="BY79">
         <v>372</v>
       </c>
+      <c r="BZ79">
+        <v>379</v>
+      </c>
     </row>
-    <row r="80" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>78</v>
       </c>
@@ -19942,8 +20179,11 @@
       <c r="BY80">
         <v>99</v>
       </c>
+      <c r="BZ80">
+        <v>102</v>
+      </c>
     </row>
-    <row r="81" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>79</v>
       </c>
@@ -20175,8 +20415,11 @@
       <c r="BY81" s="2">
         <v>113745</v>
       </c>
+      <c r="BZ81" s="2">
+        <v>115499</v>
+      </c>
     </row>
-    <row r="82" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>80</v>
       </c>
@@ -20408,8 +20651,11 @@
       <c r="BY82">
         <v>289</v>
       </c>
+      <c r="BZ82">
+        <v>298</v>
+      </c>
     </row>
-    <row r="83" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>81</v>
       </c>
@@ -20641,8 +20887,11 @@
       <c r="BY83">
         <v>2050</v>
       </c>
+      <c r="BZ83">
+        <v>2075</v>
+      </c>
     </row>
-    <row r="84" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>82</v>
       </c>
@@ -20874,8 +21123,11 @@
       <c r="BY84">
         <v>1048</v>
       </c>
+      <c r="BZ84">
+        <v>1056</v>
+      </c>
     </row>
-    <row r="85" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>83</v>
       </c>
@@ -21107,8 +21359,11 @@
       <c r="BY85">
         <v>318</v>
       </c>
+      <c r="BZ85">
+        <v>322</v>
+      </c>
     </row>
-    <row r="86" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>84</v>
       </c>
@@ -21340,8 +21595,11 @@
       <c r="BY86" s="2">
         <v>54821</v>
       </c>
+      <c r="BZ86" s="2">
+        <v>56590</v>
+      </c>
     </row>
-    <row r="87" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>85</v>
       </c>
@@ -21573,8 +21831,11 @@
       <c r="BY87">
         <v>3</v>
       </c>
+      <c r="BZ87">
+        <v>3</v>
+      </c>
     </row>
-    <row r="88" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>86</v>
       </c>
@@ -21806,8 +22067,11 @@
       <c r="BY88" s="2">
         <v>1361</v>
       </c>
+      <c r="BZ88" s="2">
+        <v>1506</v>
+      </c>
     </row>
-    <row r="89" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>87</v>
       </c>
@@ -22039,8 +22303,11 @@
       <c r="BY89">
         <v>84</v>
       </c>
+      <c r="BZ89">
+        <v>85</v>
+      </c>
     </row>
-    <row r="90" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>88</v>
       </c>
@@ -22272,8 +22539,11 @@
       <c r="BY90">
         <v>236</v>
       </c>
+      <c r="BZ90">
+        <v>248</v>
+      </c>
     </row>
-    <row r="91" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
         <v>89</v>
       </c>
@@ -22505,8 +22775,11 @@
       <c r="BY91" s="2">
         <v>1354</v>
       </c>
+      <c r="BZ91" s="2">
+        <v>1402</v>
+      </c>
     </row>
-    <row r="92" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>90</v>
       </c>
@@ -22738,8 +23011,11 @@
       <c r="BY92">
         <v>958</v>
       </c>
+      <c r="BZ92">
+        <v>960</v>
+      </c>
     </row>
-    <row r="93" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A93" s="5" t="s">
         <v>91</v>
       </c>
@@ -22971,8 +23247,11 @@
       <c r="BY93" s="2">
         <v>8998</v>
       </c>
+      <c r="BZ93" s="2">
+        <v>9077</v>
+      </c>
     </row>
-    <row r="94" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A94" s="5" t="s">
         <v>92</v>
       </c>
@@ -23204,8 +23483,11 @@
       <c r="BY94" s="2">
         <v>3593</v>
       </c>
+      <c r="BZ94" s="2">
+        <v>3911</v>
+      </c>
     </row>
-    <row r="95" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A95" s="5" t="s">
         <v>93</v>
       </c>
@@ -23437,8 +23719,11 @@
       <c r="BY95" s="2">
         <v>2824</v>
       </c>
+      <c r="BZ95" s="2">
+        <v>2850</v>
+      </c>
     </row>
-    <row r="96" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>94</v>
       </c>
@@ -23670,8 +23955,11 @@
       <c r="BY96" s="2">
         <v>5151</v>
       </c>
+      <c r="BZ96" s="2">
+        <v>5428</v>
+      </c>
     </row>
-    <row r="97" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A97" s="5" t="s">
         <v>95</v>
       </c>
@@ -23903,8 +24191,11 @@
       <c r="BY97">
         <v>731</v>
       </c>
+      <c r="BZ97">
+        <v>741</v>
+      </c>
     </row>
-    <row r="98" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A98" s="5" t="s">
         <v>96</v>
       </c>
@@ -24136,8 +24427,11 @@
       <c r="BY98">
         <v>166</v>
       </c>
+      <c r="BZ98">
+        <v>166</v>
+      </c>
     </row>
-    <row r="99" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A99" s="5" t="s">
         <v>97</v>
       </c>
@@ -24369,8 +24663,11 @@
       <c r="BY99">
         <v>865</v>
       </c>
+      <c r="BZ99">
+        <v>866</v>
+      </c>
     </row>
-    <row r="100" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A100" s="5" t="s">
         <v>98</v>
       </c>
@@ -24602,8 +24899,11 @@
       <c r="BY100">
         <v>59</v>
       </c>
+      <c r="BZ100">
+        <v>60</v>
+      </c>
     </row>
-    <row r="101" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A101" s="5" t="s">
         <v>99</v>
       </c>
@@ -24835,8 +25135,11 @@
       <c r="BY101">
         <v>84</v>
       </c>
+      <c r="BZ101">
+        <v>89</v>
+      </c>
     </row>
-    <row r="102" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A102" s="5" t="s">
         <v>100</v>
       </c>
@@ -25068,8 +25371,11 @@
       <c r="BY102" s="2">
         <v>1261</v>
       </c>
+      <c r="BZ102" s="2">
+        <v>1467</v>
+      </c>
     </row>
-    <row r="103" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
         <v>101</v>
       </c>
@@ -25301,8 +25607,11 @@
       <c r="BY103" s="2">
         <v>342489</v>
       </c>
+      <c r="BZ103" s="2">
+        <v>351760</v>
+      </c>
     </row>
-    <row r="104" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
         <v>102</v>
       </c>
@@ -25534,8 +25843,11 @@
       <c r="BY104" s="2">
         <v>5449</v>
       </c>
+      <c r="BZ104" s="2">
+        <v>5633</v>
+      </c>
     </row>
-    <row r="105" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A105" s="5" t="s">
         <v>103</v>
       </c>
@@ -25767,8 +26079,11 @@
       <c r="BY105">
         <v>127</v>
       </c>
+      <c r="BZ105">
+        <v>128</v>
+      </c>
     </row>
-    <row r="106" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A106" s="5" t="s">
         <v>104</v>
       </c>
@@ -26000,8 +26315,11 @@
       <c r="BY106">
         <v>309</v>
       </c>
+      <c r="BZ106">
+        <v>309</v>
+      </c>
     </row>
-    <row r="107" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A107" s="5" t="s">
         <v>105</v>
       </c>
@@ -26233,8 +26551,11 @@
       <c r="BY107" s="2">
         <v>17084</v>
       </c>
+      <c r="BZ107" s="2">
+        <v>18356</v>
+      </c>
     </row>
-    <row r="108" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
         <v>106</v>
       </c>
@@ -26466,8 +26787,11 @@
       <c r="BY108">
         <v>211</v>
       </c>
+      <c r="BZ108">
+        <v>212</v>
+      </c>
     </row>
-    <row r="109" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
         <v>107</v>
       </c>
@@ -26699,8 +27023,11 @@
       <c r="BY109" s="2">
         <v>2165</v>
       </c>
+      <c r="BZ109" s="2">
+        <v>2192</v>
+      </c>
     </row>
-    <row r="110" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A110" s="5" t="s">
         <v>108</v>
       </c>
@@ -26932,8 +27259,11 @@
       <c r="BY110" s="2">
         <v>35523</v>
       </c>
+      <c r="BZ110" s="2">
+        <v>36877</v>
+      </c>
     </row>
-    <row r="111" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A111" s="5" t="s">
         <v>109</v>
       </c>
@@ -27165,8 +27495,11 @@
       <c r="BY111" s="2">
         <v>1424</v>
       </c>
+      <c r="BZ111" s="2">
+        <v>1445</v>
+      </c>
     </row>
-    <row r="112" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A112" s="5" t="s">
         <v>110</v>
       </c>
@@ -27398,8 +27731,11 @@
       <c r="BY112">
         <v>138</v>
       </c>
+      <c r="BZ112">
+        <v>138</v>
+      </c>
     </row>
-    <row r="113" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A113" s="5" t="s">
         <v>111</v>
       </c>
@@ -27631,8 +27967,11 @@
       <c r="BY113" s="2">
         <v>1506</v>
       </c>
+      <c r="BZ113" s="2">
+        <v>1523</v>
+      </c>
     </row>
-    <row r="114" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A114" s="5" t="s">
         <v>112</v>
       </c>
@@ -27864,8 +28203,11 @@
       <c r="BY114">
         <v>811</v>
       </c>
+      <c r="BZ114">
+        <v>818</v>
+      </c>
     </row>
-    <row r="115" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A115" s="5" t="s">
         <v>113</v>
       </c>
@@ -28097,8 +28439,11 @@
       <c r="BY115" s="2">
         <v>3172</v>
       </c>
+      <c r="BZ115" s="2">
+        <v>3178</v>
+      </c>
     </row>
-    <row r="116" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A116" s="5" t="s">
         <v>114</v>
       </c>
@@ -28330,8 +28675,11 @@
       <c r="BY116">
         <v>685</v>
       </c>
+      <c r="BZ116">
+        <v>698</v>
+      </c>
     </row>
-    <row r="117" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A117" s="5" t="s">
         <v>115</v>
       </c>
@@ -28563,8 +28911,11 @@
       <c r="BY117">
         <v>64</v>
       </c>
+      <c r="BZ117">
+        <v>65</v>
+      </c>
     </row>
-    <row r="118" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
         <v>116</v>
       </c>
@@ -28796,8 +29147,11 @@
       <c r="BY118" s="2">
         <v>4350</v>
       </c>
+      <c r="BZ118" s="2">
+        <v>4403</v>
+      </c>
     </row>
-    <row r="119" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
         <v>117</v>
       </c>
@@ -29029,8 +29383,11 @@
       <c r="BY119">
         <v>703</v>
       </c>
+      <c r="BZ119">
+        <v>704</v>
+      </c>
     </row>
-    <row r="120" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
         <v>118</v>
       </c>
@@ -29262,8 +29619,11 @@
       <c r="BY120">
         <v>11</v>
       </c>
+      <c r="BZ120">
+        <v>12</v>
+      </c>
     </row>
-    <row r="121" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
         <v>119</v>
       </c>
@@ -29495,8 +29855,11 @@
       <c r="BY121">
         <v>119</v>
       </c>
+      <c r="BZ121">
+        <v>119</v>
+      </c>
     </row>
-    <row r="122" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
         <v>120</v>
       </c>
@@ -29728,8 +30091,11 @@
       <c r="BY122">
         <v>994</v>
       </c>
+      <c r="BZ122">
+        <v>1066</v>
+      </c>
     </row>
-    <row r="123" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
         <v>121</v>
       </c>
@@ -29961,8 +30327,11 @@
       <c r="BY123" s="2">
         <v>1185</v>
       </c>
+      <c r="BZ123" s="2">
+        <v>1355</v>
+      </c>
     </row>
-    <row r="124" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A124" s="5" t="s">
         <v>122</v>
       </c>
@@ -30194,8 +30563,11 @@
       <c r="BY124">
         <v>19</v>
       </c>
+      <c r="BZ124">
+        <v>22</v>
+      </c>
     </row>
-    <row r="125" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A125" s="5" t="s">
         <v>123</v>
       </c>
@@ -30427,8 +30799,11 @@
       <c r="BY125" s="2">
         <v>23071</v>
       </c>
+      <c r="BZ125" s="2">
+        <v>23465</v>
+      </c>
     </row>
-    <row r="126" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A126" s="5" t="s">
         <v>124</v>
       </c>
@@ -30660,8 +31035,11 @@
       <c r="BY126">
         <v>355</v>
       </c>
+      <c r="BZ126">
+        <v>376</v>
+      </c>
     </row>
-    <row r="127" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A127" s="5" t="s">
         <v>125</v>
       </c>
@@ -30893,8 +31271,11 @@
       <c r="BY127" s="2">
         <v>2872</v>
       </c>
+      <c r="BZ127" s="2">
+        <v>3019</v>
+      </c>
     </row>
-    <row r="128" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A128" s="5" t="s">
         <v>126</v>
       </c>
@@ -31126,8 +31507,11 @@
       <c r="BY128" s="2">
         <v>9958</v>
       </c>
+      <c r="BZ128" s="2">
+        <v>10255</v>
+      </c>
     </row>
-    <row r="129" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A129" s="5" t="s">
         <v>127</v>
       </c>
@@ -31359,8 +31743,11 @@
       <c r="BY129">
         <v>773</v>
       </c>
+      <c r="BZ129">
+        <v>774</v>
+      </c>
     </row>
-    <row r="130" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A130" s="5" t="s">
         <v>128</v>
       </c>
@@ -31592,8 +31979,11 @@
       <c r="BY130">
         <v>764</v>
       </c>
+      <c r="BZ130">
+        <v>780</v>
+      </c>
     </row>
-    <row r="131" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A131" s="5" t="s">
         <v>129</v>
       </c>
@@ -31825,8 +32215,11 @@
       <c r="BY131" s="2">
         <v>6132</v>
       </c>
+      <c r="BZ131" s="2">
+        <v>6239</v>
+      </c>
     </row>
-    <row r="132" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A132" s="5" t="s">
         <v>130</v>
       </c>
@@ -32058,8 +32451,11 @@
       <c r="BY132" s="2">
         <v>1737</v>
       </c>
+      <c r="BZ132" s="2">
+        <v>1851</v>
+      </c>
     </row>
-    <row r="133" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>131</v>
       </c>
@@ -32291,8 +32687,11 @@
       <c r="BY133">
         <v>5</v>
       </c>
+      <c r="BZ133">
+        <v>5</v>
+      </c>
     </row>
-    <row r="134" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A134" s="5" t="s">
         <v>132</v>
       </c>
@@ -32524,8 +32923,11 @@
       <c r="BY134">
         <v>3</v>
       </c>
+      <c r="BZ134">
+        <v>3</v>
+      </c>
     </row>
-    <row r="135" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A135" s="5" t="s">
         <v>133</v>
       </c>
@@ -32757,8 +33159,11 @@
       <c r="BY135" s="2">
         <v>3026</v>
       </c>
+      <c r="BZ135" s="2">
+        <v>3277</v>
+      </c>
     </row>
-    <row r="136" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A136" s="5" t="s">
         <v>134</v>
       </c>
@@ -32990,8 +33395,11 @@
       <c r="BY136">
         <v>132</v>
       </c>
+      <c r="BZ136">
+        <v>137</v>
+      </c>
     </row>
-    <row r="137" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A137" s="5" t="s">
         <v>135</v>
       </c>
@@ -33223,8 +33631,11 @@
       <c r="BY137">
         <v>5</v>
       </c>
+      <c r="BZ137">
+        <v>5</v>
+      </c>
     </row>
-    <row r="138" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A138" s="5" t="s">
         <v>136</v>
       </c>
@@ -33456,8 +33867,11 @@
       <c r="BY138">
         <v>32</v>
       </c>
+      <c r="BZ138">
+        <v>33</v>
+      </c>
     </row>
-    <row r="139" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A139" s="5" t="s">
         <v>137</v>
       </c>
@@ -33689,8 +34103,11 @@
       <c r="BY139" s="2">
         <v>2806</v>
       </c>
+      <c r="BZ139" s="2">
+        <v>2820</v>
+      </c>
     </row>
-    <row r="140" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A140" s="5" t="s">
         <v>138</v>
       </c>
@@ -33922,8 +34339,11 @@
       <c r="BY140">
         <v>212</v>
       </c>
+      <c r="BZ140">
+        <v>224</v>
+      </c>
     </row>
-    <row r="141" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A141" s="5" t="s">
         <v>139</v>
       </c>
@@ -34155,8 +34575,11 @@
       <c r="BY141" s="2">
         <v>1513</v>
       </c>
+      <c r="BZ141" s="2">
+        <v>1527</v>
+      </c>
     </row>
-    <row r="142" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A142" s="5" t="s">
         <v>140</v>
       </c>
@@ -34388,8 +34811,11 @@
       <c r="BY142">
         <v>300</v>
       </c>
+      <c r="BZ142">
+        <v>300</v>
+      </c>
     </row>
-    <row r="143" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A143" s="5" t="s">
         <v>141</v>
       </c>
@@ -34621,8 +35047,11 @@
       <c r="BY143" s="2">
         <v>1695</v>
       </c>
+      <c r="BZ143" s="2">
+        <v>1703</v>
+      </c>
     </row>
-    <row r="144" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A144" s="5" t="s">
         <v>142</v>
       </c>
@@ -34854,8 +35283,11 @@
       <c r="BY144">
         <v>625</v>
       </c>
+      <c r="BZ144">
+        <v>632</v>
+      </c>
     </row>
-    <row r="145" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A145" s="5" t="s">
         <v>143</v>
       </c>
@@ -35087,8 +35519,11 @@
       <c r="BY145">
         <v>1029</v>
       </c>
+      <c r="BZ145">
+        <v>1266</v>
+      </c>
     </row>
-    <row r="146" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A146" s="5" t="s">
         <v>144</v>
       </c>
@@ -35320,8 +35755,11 @@
       <c r="BY146">
         <v>809</v>
       </c>
+      <c r="BZ146">
+        <v>1142</v>
+      </c>
     </row>
-    <row r="147" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A147" s="5" t="s">
         <v>145</v>
       </c>
@@ -35553,8 +35991,11 @@
       <c r="BY147">
         <v>783</v>
       </c>
+      <c r="BZ147">
+        <v>986</v>
+      </c>
     </row>
-    <row r="148" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A148" s="5" t="s">
         <v>146</v>
       </c>
@@ -35786,8 +36227,11 @@
       <c r="BY148" s="2">
         <v>5321</v>
       </c>
+      <c r="BZ148" s="2">
+        <v>5438</v>
+      </c>
     </row>
-    <row r="149" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A149" s="5" t="s">
         <v>147</v>
       </c>
@@ -36019,8 +36463,11 @@
       <c r="BY149">
         <v>1261</v>
       </c>
+      <c r="BZ149">
+        <v>1278</v>
+      </c>
     </row>
-    <row r="150" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A150" s="5" t="s">
         <v>148</v>
       </c>
@@ -36252,8 +36699,11 @@
       <c r="BY150">
         <v>124</v>
       </c>
+      <c r="BZ150">
+        <v>124</v>
+      </c>
     </row>
-    <row r="151" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A151" s="5" t="s">
         <v>149</v>
       </c>
@@ -36485,8 +36935,11 @@
       <c r="BY151">
         <v>518</v>
       </c>
+      <c r="BZ151">
+        <v>534</v>
+      </c>
     </row>
-    <row r="152" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A152" s="5" t="s">
         <v>150</v>
       </c>
@@ -36718,8 +37171,11 @@
       <c r="BY152" s="2">
         <v>1250</v>
       </c>
+      <c r="BZ152" s="2">
+        <v>1272</v>
+      </c>
     </row>
-    <row r="153" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A153" s="5" t="s">
         <v>151</v>
       </c>
@@ -36951,8 +37407,11 @@
       <c r="BY153">
         <v>1</v>
       </c>
+      <c r="BZ153">
+        <v>1</v>
+      </c>
     </row>
-    <row r="154" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A154" s="5" t="s">
         <v>152</v>
       </c>
@@ -37184,8 +37643,11 @@
       <c r="BY154" s="2">
         <v>17260</v>
       </c>
+      <c r="BZ154" s="2">
+        <v>17410</v>
+      </c>
     </row>
-    <row r="155" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A155" s="5" t="s">
         <v>153</v>
       </c>
@@ -37417,8 +37879,11 @@
       <c r="BY155">
         <v>549</v>
       </c>
+      <c r="BZ155">
+        <v>556</v>
+      </c>
     </row>
-    <row r="156" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A156" s="5" t="s">
         <v>154</v>
       </c>
@@ -37650,8 +38115,11 @@
       <c r="BY156">
         <v>137</v>
       </c>
+      <c r="BZ156">
+        <v>146</v>
+      </c>
     </row>
-    <row r="157" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A157" s="5" t="s">
         <v>155</v>
       </c>
@@ -37883,8 +38351,11 @@
       <c r="BY157" s="2">
         <v>17180</v>
       </c>
+      <c r="BZ157" s="2">
+        <v>17890</v>
+      </c>
     </row>
-    <row r="158" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A158" s="5" t="s">
         <v>156</v>
       </c>
@@ -38116,8 +38587,11 @@
       <c r="BY158">
         <v>23</v>
       </c>
+      <c r="BZ158">
+        <v>23</v>
+      </c>
     </row>
-    <row r="159" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A159" s="5" t="s">
         <v>157</v>
       </c>
@@ -38349,8 +38823,11 @@
       <c r="BY159">
         <v>2908</v>
       </c>
+      <c r="BZ159">
+        <v>2960</v>
+      </c>
     </row>
-    <row r="160" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A160" s="5" t="s">
         <v>158</v>
       </c>
@@ -38582,8 +39059,11 @@
       <c r="BY160">
         <v>136</v>
       </c>
+      <c r="BZ160">
+        <v>137</v>
+      </c>
     </row>
-    <row r="161" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A161" s="5" t="s">
         <v>159</v>
       </c>
@@ -38815,8 +39295,11 @@
       <c r="BY161">
         <v>131</v>
       </c>
+      <c r="BZ161">
+        <v>135</v>
+      </c>
     </row>
-    <row r="162" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A162" s="5" t="s">
         <v>160</v>
       </c>
@@ -39048,8 +39531,11 @@
       <c r="BY162">
         <v>378</v>
       </c>
+      <c r="BZ162">
+        <v>378</v>
+      </c>
     </row>
-    <row r="163" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A163" s="5" t="s">
         <v>161</v>
       </c>
@@ -39281,8 +39767,11 @@
       <c r="BY163" s="2">
         <v>2739</v>
       </c>
+      <c r="BZ163" s="2">
+        <v>2804</v>
+      </c>
     </row>
-    <row r="164" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A164" s="5" t="s">
         <v>162</v>
       </c>
@@ -39514,8 +40003,11 @@
       <c r="BY164" s="2">
         <v>5115</v>
       </c>
+      <c r="BZ164" s="2">
+        <v>5207</v>
+      </c>
     </row>
-    <row r="165" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A165" s="5" t="s">
         <v>163</v>
       </c>
@@ -39747,8 +40239,11 @@
       <c r="BY165" s="2">
         <v>3046</v>
       </c>
+      <c r="BZ165" s="2">
+        <v>3067</v>
+      </c>
     </row>
-    <row r="166" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A166" s="5" t="s">
         <v>164</v>
       </c>
@@ -39980,8 +40475,11 @@
       <c r="BY166">
         <v>72</v>
       </c>
+      <c r="BZ166">
+        <v>74</v>
+      </c>
     </row>
-    <row r="167" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A167" s="5" t="s">
         <v>165</v>
       </c>
@@ -40213,8 +40711,11 @@
       <c r="BY167" s="2">
         <v>7368</v>
       </c>
+      <c r="BZ167" s="2">
+        <v>7564</v>
+      </c>
     </row>
-    <row r="168" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A168" s="5" t="s">
         <v>166</v>
       </c>
@@ -40446,8 +40947,11 @@
       <c r="BY168" s="2">
         <v>1748</v>
       </c>
+      <c r="BZ168" s="2">
+        <v>1872</v>
+      </c>
     </row>
-    <row r="169" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A169" s="5" t="s">
         <v>167</v>
       </c>
@@ -40679,8 +41183,11 @@
       <c r="BY169">
         <v>119</v>
       </c>
+      <c r="BZ169">
+        <v>120</v>
+      </c>
     </row>
-    <row r="170" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A170" s="5" t="s">
         <v>168</v>
       </c>
@@ -40912,8 +41419,11 @@
       <c r="BY170">
         <v>267</v>
       </c>
+      <c r="BZ170">
+        <v>269</v>
+      </c>
     </row>
-    <row r="171" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A171" s="5" t="s">
         <v>169</v>
       </c>
@@ -41145,8 +41655,11 @@
       <c r="BY171">
         <v>381</v>
       </c>
+      <c r="BZ171">
+        <v>393</v>
+      </c>
     </row>
-    <row r="172" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A172" s="5" t="s">
         <v>170</v>
       </c>
@@ -41378,8 +41891,11 @@
       <c r="BY172" s="2">
         <v>35864</v>
       </c>
+      <c r="BZ172" s="2">
+        <v>36715</v>
+      </c>
     </row>
-    <row r="173" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A173" s="5" t="s">
         <v>171</v>
       </c>
@@ -41611,8 +42127,11 @@
       <c r="BY173" s="2">
         <v>3158</v>
       </c>
+      <c r="BZ173" s="2">
+        <v>3162</v>
+      </c>
     </row>
-    <row r="174" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A174" s="5" t="s">
         <v>172</v>
       </c>
@@ -41844,8 +42363,11 @@
       <c r="BY174">
         <v>303</v>
       </c>
+      <c r="BZ174">
+        <v>322</v>
+      </c>
     </row>
-    <row r="175" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A175" s="5" t="s">
         <v>173</v>
       </c>
@@ -42077,8 +42599,11 @@
       <c r="BY175">
         <v>35</v>
       </c>
+      <c r="BZ175">
+        <v>35</v>
+      </c>
     </row>
-    <row r="176" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A176" s="5" t="s">
         <v>174</v>
       </c>
@@ -42310,8 +42835,11 @@
       <c r="BY176" s="2">
         <v>3973</v>
       </c>
+      <c r="BZ176" s="2">
+        <v>4008</v>
+      </c>
     </row>
-    <row r="177" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A177" s="5" t="s">
         <v>175</v>
       </c>
@@ -42543,8 +43071,11 @@
       <c r="BY177" s="2">
         <v>1901</v>
       </c>
+      <c r="BZ177" s="2">
+        <v>1908</v>
+      </c>
     </row>
-    <row r="178" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A178" s="5" t="s">
         <v>176</v>
       </c>
@@ -42776,8 +43307,11 @@
       <c r="BY178">
         <v>367</v>
       </c>
+      <c r="BZ178">
+        <v>412</v>
+      </c>
     </row>
-    <row r="179" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A179" s="5" t="s">
         <v>177</v>
       </c>
@@ -43009,8 +43543,11 @@
       <c r="BY179">
         <v>216</v>
       </c>
+      <c r="BZ179">
+        <v>223</v>
+      </c>
     </row>
-    <row r="180" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A180" s="5" t="s">
         <v>178</v>
       </c>
@@ -43242,8 +43779,11 @@
       <c r="BY180" s="2">
         <v>10421</v>
       </c>
+      <c r="BZ180" s="2">
+        <v>10936</v>
+      </c>
     </row>
-    <row r="181" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A181" s="5" t="s">
         <v>179</v>
       </c>
@@ -43475,8 +44015,11 @@
       <c r="BY181">
         <v>157</v>
       </c>
+      <c r="BZ181">
+        <v>158</v>
+      </c>
     </row>
-    <row r="182" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A182" s="5" t="s">
         <v>180</v>
       </c>
@@ -43708,8 +44251,11 @@
       <c r="BY182">
         <v>126</v>
       </c>
+      <c r="BZ182">
+        <v>126</v>
+      </c>
     </row>
-    <row r="183" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A183" s="5" t="s">
         <v>181</v>
       </c>
@@ -43941,8 +44487,11 @@
       <c r="BY183" s="2">
         <v>2250</v>
       </c>
+      <c r="BZ183" s="2">
+        <v>2339</v>
+      </c>
     </row>
-    <row r="184" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A184" s="5" t="s">
         <v>182</v>
       </c>
@@ -44174,8 +44723,11 @@
       <c r="BY184">
         <v>702</v>
       </c>
+      <c r="BZ184">
+        <v>706</v>
+      </c>
     </row>
-    <row r="185" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A185" s="5" t="s">
         <v>183</v>
       </c>
@@ -44407,8 +44959,11 @@
       <c r="BY185">
         <v>757</v>
       </c>
+      <c r="BZ185">
+        <v>778</v>
+      </c>
     </row>
-    <row r="186" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A186" s="5" t="s">
         <v>184</v>
       </c>
@@ -44640,8 +45195,11 @@
       <c r="BY186" s="2">
         <v>7495</v>
       </c>
+      <c r="BZ186" s="2">
+        <v>7590</v>
+      </c>
     </row>
-    <row r="187" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A187" s="5" t="s">
         <v>185</v>
       </c>
@@ -44873,8 +45431,11 @@
       <c r="BY187">
         <v>346</v>
       </c>
+      <c r="BZ187">
+        <v>346</v>
+      </c>
     </row>
-    <row r="188" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A188" s="5" t="s">
         <v>186</v>
       </c>
@@ -45106,8 +45667,11 @@
       <c r="BY188" s="2">
         <v>1995</v>
       </c>
+      <c r="BZ188" s="2">
+        <v>1996</v>
+      </c>
     </row>
-    <row r="189" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A189" s="5" t="s">
         <v>187</v>
       </c>
@@ -45339,8 +45903,11 @@
       <c r="BY189" s="2">
         <v>3281</v>
       </c>
+      <c r="BZ189" s="2">
+        <v>3323</v>
+      </c>
     </row>
-    <row r="190" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A190" s="5" t="s">
         <v>188</v>
       </c>
@@ -45572,8 +46139,11 @@
       <c r="BY190" s="2">
         <v>16864</v>
       </c>
+      <c r="BZ190" s="2">
+        <v>16903</v>
+      </c>
     </row>
-    <row r="191" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A191" s="5" t="s">
         <v>189</v>
       </c>
@@ -45805,8 +46375,11 @@
       <c r="BY191">
         <v>145</v>
       </c>
+      <c r="BZ191">
+        <v>323</v>
+      </c>
     </row>
-    <row r="192" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A192" s="5" t="s">
         <v>190</v>
       </c>
@@ -46038,8 +46611,11 @@
       <c r="BY192">
         <v>168</v>
       </c>
+      <c r="BZ192">
+        <v>171</v>
+      </c>
     </row>
-    <row r="193" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A193" s="5" t="s">
         <v>191</v>
       </c>
@@ -46271,8 +46847,11 @@
       <c r="BY193" s="2">
         <v>5886</v>
       </c>
+      <c r="BZ193" s="2">
+        <v>5937</v>
+      </c>
     </row>
-    <row r="194" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A194" s="5" t="s">
         <v>192</v>
       </c>
@@ -46504,8 +47083,11 @@
       <c r="BY194">
         <v>122</v>
       </c>
+      <c r="BZ194">
+        <v>122</v>
+      </c>
     </row>
-    <row r="195" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A195" s="5" t="s">
         <v>193</v>
       </c>
@@ -46737,8 +47319,11 @@
       <c r="BY195">
         <v>151</v>
       </c>
+      <c r="BZ195">
+        <v>151</v>
+      </c>
     </row>
-    <row r="196" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A196" s="5" t="s">
         <v>194</v>
       </c>
@@ -46970,8 +47555,11 @@
       <c r="BY196">
         <v>529</v>
       </c>
+      <c r="BZ196">
+        <v>531</v>
+      </c>
     </row>
-    <row r="197" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A197" s="5" t="s">
         <v>195</v>
       </c>
@@ -47203,8 +47791,11 @@
       <c r="BY197">
         <v>315</v>
       </c>
+      <c r="BZ197">
+        <v>317</v>
+      </c>
     </row>
-    <row r="198" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A198" s="5" t="s">
         <v>196</v>
       </c>
@@ -47436,8 +48027,11 @@
       <c r="BY198">
         <v>276</v>
       </c>
+      <c r="BZ198">
+        <v>280</v>
+      </c>
     </row>
-    <row r="199" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A199" s="5" t="s">
         <v>197</v>
       </c>
@@ -47669,8 +48263,11 @@
       <c r="BY199">
         <v>12</v>
       </c>
+      <c r="BZ199">
+        <v>13</v>
+      </c>
     </row>
-    <row r="200" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A200" s="5" t="s">
         <v>198</v>
       </c>
@@ -47902,8 +48499,11 @@
       <c r="BY200">
         <v>864</v>
       </c>
+      <c r="BZ200">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="201" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A201" s="5" t="s">
         <v>199</v>
       </c>
@@ -48135,8 +48735,11 @@
       <c r="BY201" s="2">
         <v>5926</v>
       </c>
+      <c r="BZ201" s="2">
+        <v>6028</v>
+      </c>
     </row>
-    <row r="202" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A202" s="5" t="s">
         <v>200</v>
       </c>
@@ -48368,8 +48971,11 @@
       <c r="BY202">
         <v>400</v>
       </c>
+      <c r="BZ202">
+        <v>416</v>
+      </c>
     </row>
-    <row r="203" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A203" s="5" t="s">
         <v>201</v>
       </c>
@@ -48601,8 +49207,11 @@
       <c r="BY203" s="2">
         <v>4452</v>
       </c>
+      <c r="BZ203" s="2">
+        <v>4505</v>
+      </c>
     </row>
-    <row r="204" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A204" s="5" t="s">
         <v>202</v>
       </c>
@@ -48834,8 +49443,11 @@
       <c r="BY204">
         <v>573</v>
       </c>
+      <c r="BZ204">
+        <v>589</v>
+      </c>
     </row>
-    <row r="205" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A205" s="5" t="s">
         <v>203</v>
       </c>
@@ -49067,8 +49679,11 @@
       <c r="BY205">
         <v>415</v>
       </c>
+      <c r="BZ205">
+        <v>427</v>
+      </c>
     </row>
-    <row r="206" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A206" s="5" t="s">
         <v>204</v>
       </c>
@@ -49300,8 +49915,11 @@
       <c r="BY206">
         <v>877</v>
       </c>
+      <c r="BZ206">
+        <v>890</v>
+      </c>
     </row>
-    <row r="207" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A207" s="5" t="s">
         <v>205</v>
       </c>
@@ -49533,8 +50151,11 @@
       <c r="BY207" s="2">
         <v>1728</v>
       </c>
+      <c r="BZ207" s="2">
+        <v>1784</v>
+      </c>
     </row>
-    <row r="208" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A208" s="5" t="s">
         <v>206</v>
       </c>
@@ -49766,8 +50387,11 @@
       <c r="BY208">
         <v>206</v>
       </c>
+      <c r="BZ208">
+        <v>208</v>
+      </c>
     </row>
-    <row r="209" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A209" s="5" t="s">
         <v>207</v>
       </c>
@@ -49999,8 +50623,11 @@
       <c r="BY209">
         <v>136</v>
       </c>
+      <c r="BZ209">
+        <v>140</v>
+      </c>
     </row>
-    <row r="210" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A210" s="5" t="s">
         <v>208</v>
       </c>
@@ -50232,8 +50859,11 @@
       <c r="BY210">
         <v>112</v>
       </c>
+      <c r="BZ210">
+        <v>112</v>
+      </c>
     </row>
-    <row r="211" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A211" s="5" t="s">
         <v>209</v>
       </c>
@@ -50465,8 +51095,11 @@
       <c r="BY211">
         <v>50</v>
       </c>
+      <c r="BZ211">
+        <v>50</v>
+      </c>
     </row>
-    <row r="212" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A212" s="5" t="s">
         <v>210</v>
       </c>
@@ -50698,8 +51331,11 @@
       <c r="BY212" s="2">
         <v>1667</v>
       </c>
+      <c r="BZ212" s="2">
+        <v>1683</v>
+      </c>
     </row>
-    <row r="213" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A213" s="5" t="s">
         <v>211</v>
       </c>
@@ -50931,8 +51567,11 @@
       <c r="BY213">
         <v>42</v>
       </c>
+      <c r="BZ213">
+        <v>42</v>
+      </c>
     </row>
-    <row r="214" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A214" s="5" t="s">
         <v>212</v>
       </c>
@@ -51164,8 +51803,11 @@
       <c r="BY214" s="2">
         <v>9736</v>
       </c>
+      <c r="BZ214" s="2">
+        <v>10536</v>
+      </c>
     </row>
-    <row r="215" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A215" s="5" t="s">
         <v>213</v>
       </c>
@@ -51397,8 +52039,11 @@
       <c r="BY215">
         <v>320</v>
       </c>
+      <c r="BZ215">
+        <v>322</v>
+      </c>
     </row>
-    <row r="216" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A216" s="5" t="s">
         <v>214</v>
       </c>
@@ -51630,8 +52275,11 @@
       <c r="BY216" s="2">
         <v>4492</v>
       </c>
+      <c r="BZ216" s="2">
+        <v>4570</v>
+      </c>
     </row>
-    <row r="217" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A217" s="5" t="s">
         <v>215</v>
       </c>
@@ -51863,8 +52511,11 @@
       <c r="BY217">
         <v>161</v>
       </c>
+      <c r="BZ217">
+        <v>166</v>
+      </c>
     </row>
-    <row r="218" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A218" s="5" t="s">
         <v>216</v>
       </c>
@@ -52096,8 +52747,11 @@
       <c r="BY218">
         <v>34</v>
       </c>
+      <c r="BZ218">
+        <v>34</v>
+      </c>
     </row>
-    <row r="219" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A219" s="5" t="s">
         <v>217</v>
       </c>
@@ -52329,8 +52983,11 @@
       <c r="BY219">
         <v>13</v>
       </c>
+      <c r="BZ219">
+        <v>13</v>
+      </c>
     </row>
-    <row r="220" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A220" s="5" t="s">
         <v>218</v>
       </c>
@@ -52562,8 +53219,11 @@
       <c r="BY220">
         <v>70</v>
       </c>
+      <c r="BZ220">
+        <v>72</v>
+      </c>
     </row>
-    <row r="221" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A221" s="5" t="s">
         <v>219</v>
       </c>
@@ -52795,8 +53455,11 @@
       <c r="BY221">
         <v>325</v>
       </c>
+      <c r="BZ221">
+        <v>330</v>
+      </c>
     </row>
-    <row r="222" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A222" s="5" t="s">
         <v>220</v>
       </c>
@@ -53028,8 +53691,11 @@
       <c r="BY222" s="2">
         <v>117759</v>
       </c>
+      <c r="BZ222" s="2">
+        <v>120120</v>
+      </c>
     </row>
-    <row r="223" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A223" s="5" t="s">
         <v>221</v>
       </c>
@@ -53261,8 +53927,11 @@
       <c r="BY223" s="2">
         <v>11076</v>
       </c>
+      <c r="BZ223" s="2">
+        <v>11150</v>
+      </c>
     </row>
-    <row r="224" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A224" s="5" t="s">
         <v>222</v>
       </c>
@@ -53494,8 +54163,11 @@
       <c r="BY224">
         <v>6</v>
       </c>
+      <c r="BZ224">
+        <v>6</v>
+      </c>
     </row>
-    <row r="225" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A225" s="5" t="s">
         <v>223</v>
       </c>
@@ -53727,8 +54399,11 @@
       <c r="BY225">
         <v>307</v>
       </c>
+      <c r="BZ225">
+        <v>308</v>
+      </c>
     </row>
-    <row r="226" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A226" s="5" t="s">
         <v>224</v>
       </c>
@@ -53960,8 +54635,11 @@
       <c r="BY226">
         <v>43</v>
       </c>
+      <c r="BZ226">
+        <v>43</v>
+      </c>
     </row>
-    <row r="227" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A227" s="5" t="s">
         <v>225</v>
       </c>
@@ -54193,8 +54871,11 @@
       <c r="BY227" s="2">
         <v>3261</v>
       </c>
+      <c r="BZ227" s="2">
+        <v>3309</v>
+      </c>
     </row>
-    <row r="228" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A228" s="5" t="s">
         <v>226</v>
       </c>
@@ -54426,8 +55107,11 @@
       <c r="BY228" s="2">
         <v>4122</v>
       </c>
+      <c r="BZ228" s="2">
+        <v>4223</v>
+      </c>
     </row>
-    <row r="229" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A229" s="5" t="s">
         <v>227</v>
       </c>
@@ -54659,8 +55343,11 @@
       <c r="BY229" s="2">
         <v>77130</v>
       </c>
+      <c r="BZ229" s="2">
+        <v>78799</v>
+      </c>
     </row>
-    <row r="230" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A230" s="5" t="s">
         <v>228</v>
       </c>
@@ -54892,8 +55579,11 @@
       <c r="BY230">
         <v>865</v>
       </c>
+      <c r="BZ230">
+        <v>910</v>
+      </c>
     </row>
-    <row r="231" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A231" s="5" t="s">
         <v>229</v>
       </c>
@@ -55125,8 +55815,11 @@
       <c r="BY231">
         <v>2568</v>
       </c>
+      <c r="BZ231">
+        <v>2581</v>
+      </c>
     </row>
-    <row r="232" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A232" s="5" t="s">
         <v>230</v>
       </c>
@@ -55358,8 +56051,11 @@
       <c r="BY232">
         <v>598</v>
       </c>
+      <c r="BZ232">
+        <v>636</v>
+      </c>
     </row>
-    <row r="233" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A233" s="5" t="s">
         <v>231</v>
       </c>
@@ -55591,8 +56287,11 @@
       <c r="BY233">
         <v>164</v>
       </c>
+      <c r="BZ233">
+        <v>164</v>
+      </c>
     </row>
-    <row r="234" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A234" s="5" t="s">
         <v>232</v>
       </c>
@@ -55824,8 +56523,11 @@
       <c r="BY234" s="2">
         <v>1154</v>
       </c>
+      <c r="BZ234" s="2">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="235" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A235" s="5" t="s">
         <v>233</v>
       </c>
@@ -56057,8 +56759,11 @@
       <c r="BY235" s="2">
         <v>2110</v>
       </c>
+      <c r="BZ235" s="2">
+        <v>2113</v>
+      </c>
     </row>
-    <row r="236" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A236" s="5" t="s">
         <v>234</v>
       </c>
@@ -56290,8 +56995,11 @@
       <c r="BY236" s="2">
         <v>1720</v>
       </c>
+      <c r="BZ236" s="2">
+        <v>1800</v>
+      </c>
     </row>
-    <row r="237" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A237" s="5" t="s">
         <v>235</v>
       </c>
@@ -56523,8 +57231,11 @@
       <c r="BY237" s="2">
         <v>5802</v>
       </c>
+      <c r="BZ237" s="2">
+        <v>5945</v>
+      </c>
     </row>
-    <row r="238" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A238" s="5" t="s">
         <v>236</v>
       </c>
@@ -56756,8 +57467,11 @@
       <c r="BY238" s="2">
         <v>20065</v>
       </c>
+      <c r="BZ238" s="2">
+        <v>20180</v>
+      </c>
     </row>
-    <row r="239" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A239" s="5" t="s">
         <v>237</v>
       </c>
@@ -56989,8 +57703,11 @@
       <c r="BY239" s="2">
         <v>2439</v>
       </c>
+      <c r="BZ239" s="2">
+        <v>2497</v>
+      </c>
     </row>
-    <row r="240" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A240" s="5" t="s">
         <v>238</v>
       </c>
@@ -57222,8 +57939,11 @@
       <c r="BY240">
         <v>283</v>
       </c>
+      <c r="BZ240">
+        <v>286</v>
+      </c>
     </row>
-    <row r="241" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A241" s="5" t="s">
         <v>239</v>
       </c>
@@ -57455,8 +58175,11 @@
       <c r="BY241" s="2">
         <v>2833</v>
       </c>
+      <c r="BZ241" s="2">
+        <v>2843</v>
+      </c>
     </row>
-    <row r="242" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A242" s="5" t="s">
         <v>240</v>
       </c>
@@ -57688,8 +58411,11 @@
       <c r="BY242" s="2">
         <v>11298</v>
       </c>
+      <c r="BZ242" s="2">
+        <v>11514</v>
+      </c>
     </row>
-    <row r="243" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A243" s="5" t="s">
         <v>241</v>
       </c>
@@ -57921,8 +58647,11 @@
       <c r="BY243" s="2">
         <v>2895</v>
       </c>
+      <c r="BZ243" s="2">
+        <v>2931</v>
+      </c>
     </row>
-    <row r="244" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A244" s="5" t="s">
         <v>242</v>
       </c>
@@ -58154,8 +58883,11 @@
       <c r="BY244">
         <v>152</v>
       </c>
+      <c r="BZ244">
+        <v>155</v>
+      </c>
     </row>
-    <row r="245" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A245" s="5" t="s">
         <v>243</v>
       </c>
@@ -58387,8 +59119,11 @@
       <c r="BY245" s="2">
         <v>8514</v>
       </c>
+      <c r="BZ245" s="2">
+        <v>8681</v>
+      </c>
     </row>
-    <row r="246" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A246" s="5" t="s">
         <v>244</v>
       </c>
@@ -58620,8 +59355,11 @@
       <c r="BY246">
         <v>408</v>
       </c>
+      <c r="BZ246">
+        <v>417</v>
+      </c>
     </row>
-    <row r="247" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A247" s="5" t="s">
         <v>245</v>
       </c>
@@ -58853,8 +59591,11 @@
       <c r="BY247" s="2">
         <v>2265</v>
       </c>
+      <c r="BZ247" s="2">
+        <v>2291</v>
+      </c>
     </row>
-    <row r="248" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A248" s="5" t="s">
         <v>246</v>
       </c>
@@ -59086,8 +59827,11 @@
       <c r="BY248" s="2">
         <v>25281</v>
       </c>
+      <c r="BZ248" s="2">
+        <v>25805</v>
+      </c>
     </row>
-    <row r="249" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A249" s="5" t="s">
         <v>247</v>
       </c>
@@ -59319,8 +60063,11 @@
       <c r="BY249" s="2">
         <v>1758</v>
       </c>
+      <c r="BZ249" s="2">
+        <v>1788</v>
+      </c>
     </row>
-    <row r="250" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A250" s="5" t="s">
         <v>248</v>
       </c>
@@ -59552,8 +60299,11 @@
       <c r="BY250">
         <v>50</v>
       </c>
+      <c r="BZ250">
+        <v>52</v>
+      </c>
     </row>
-    <row r="251" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A251" s="5" t="s">
         <v>249</v>
       </c>
@@ -59785,8 +60535,11 @@
       <c r="BY251" s="2">
         <v>2230</v>
       </c>
+      <c r="BZ251" s="2">
+        <v>2296</v>
+      </c>
     </row>
-    <row r="252" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A252" s="5" t="s">
         <v>250</v>
       </c>
@@ -60018,8 +60771,11 @@
       <c r="BY252">
         <v>1004</v>
       </c>
+      <c r="BZ252">
+        <v>1033</v>
+      </c>
     </row>
-    <row r="253" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A253" s="5" t="s">
         <v>251</v>
       </c>
@@ -60251,8 +61007,11 @@
       <c r="BY253">
         <v>344</v>
       </c>
+      <c r="BZ253">
+        <v>365</v>
+      </c>
     </row>
-    <row r="254" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A254" s="5" t="s">
         <v>252</v>
       </c>
@@ -60484,8 +61243,11 @@
       <c r="BY254">
         <v>767</v>
       </c>
+      <c r="BZ254">
+        <v>767</v>
+      </c>
     </row>
-    <row r="255" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A255" s="5" t="s">
         <v>253</v>
       </c>
@@ -60717,8 +61479,11 @@
       <c r="BY255">
         <v>819</v>
       </c>
+      <c r="BZ255">
+        <v>934</v>
+      </c>
     </row>
-    <row r="256" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A256" s="5" t="s">
         <v>254</v>
       </c>
@@ -60950,8 +61715,11 @@
       <c r="BY256">
         <v>467</v>
       </c>
+      <c r="BZ256">
+        <v>520</v>
+      </c>
     </row>
-    <row r="257" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A257" s="5" t="s">
         <v>255</v>
       </c>
@@ -61183,8 +61951,11 @@
       <c r="BY257" s="2">
         <v>5358</v>
       </c>
+      <c r="BZ257" s="2">
+        <v>5381</v>
+      </c>
     </row>
-    <row r="258" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A258" s="5" t="s">
         <v>256</v>
       </c>
@@ -61417,8 +62188,11 @@
       <c r="BY258" s="2">
         <v>536385</v>
       </c>
+      <c r="BZ258" s="2">
+        <v>551854</v>
+      </c>
     </row>
-    <row r="259" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A259" s="9" t="s">
         <v>257</v>
       </c>
@@ -61664,8 +62438,12 @@
         <f>SUM(BY3:BY258)</f>
         <v>2371709</v>
       </c>
+      <c r="BZ259" s="10">
+        <f>SUM(BZ3:BZ258)</f>
+        <v>2431861</v>
+      </c>
     </row>
-    <row r="261" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A261" s="3" t="s">
         <v>261</v>
       </c>
@@ -61678,7 +62456,7 @@
       <c r="H261" s="4"/>
       <c r="I261" s="4"/>
     </row>
-    <row r="262" spans="1:77" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:78" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="21" t="s">
         <v>258</v>
       </c>
@@ -61691,7 +62469,7 @@
       <c r="H262" s="22"/>
       <c r="I262" s="22"/>
     </row>
-    <row r="263" spans="1:77" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:78" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="23" t="s">
         <v>259</v>
       </c>
@@ -61704,7 +62482,7 @@
       <c r="H263" s="24"/>
       <c r="I263" s="24"/>
     </row>
-    <row r="264" spans="1:77" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:78" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="23" t="s">
         <v>260</v>
       </c>
@@ -61717,7 +62495,7 @@
       <c r="H264" s="24"/>
       <c r="I264" s="24"/>
     </row>
-    <row r="265" spans="1:77" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:78" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="11" t="s">
         <v>288</v>
       </c>
@@ -61792,9 +62570,9 @@
       <c r="BR265" s="13"/>
       <c r="BS265" s="13"/>
     </row>
-    <row r="266" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B266" s="18"/>
       <c r="C266" s="13"/>
@@ -61805,7 +62583,7 @@
       <c r="H266" s="13"/>
       <c r="I266" s="13"/>
     </row>
-    <row r="267" spans="1:77" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:78" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="23" t="s">
         <v>278</v>
       </c>

</xml_diff>